<commit_message>
added chinesische Kartoffelsuppe and added standard quantity for 4 servings for the excel tables.
</commit_message>
<xml_diff>
--- a/tbl/bun-rieu.xlsx
+++ b/tbl/bun-rieu.xlsx
@@ -222,10 +222,10 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.14"/>
   </cols>
@@ -255,7 +255,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -272,7 +272,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -289,7 +289,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>160</v>
+        <v>500</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -306,7 +306,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -323,7 +323,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -340,7 +340,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -357,7 +357,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -374,7 +374,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -391,7 +391,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -408,7 +408,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
@@ -425,7 +425,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -442,7 +442,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -459,7 +459,7 @@
         <v>24</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -476,7 +476,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -493,9 +493,9 @@
         <v>26</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">

</xml_diff>

<commit_message>
Zutaten angepasst bun rieu
</commit_message>
<xml_diff>
--- a/tbl/bun-rieu.xlsx
+++ b/tbl/bun-rieu.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Stück</t>
   </si>
   <si>
-    <t xml:space="preserve">Eier (M)</t>
+    <t xml:space="preserve">Eier (L)</t>
   </si>
   <si>
     <t xml:space="preserve">Wasser</t>
@@ -73,13 +73,10 @@
     <t xml:space="preserve">Öl</t>
   </si>
   <si>
-    <t xml:space="preserve">Teelöffel</t>
+    <t xml:space="preserve">Esslöffel</t>
   </si>
   <si>
     <t xml:space="preserve">Fischsoße</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esslöffel</t>
   </si>
   <si>
     <t xml:space="preserve">Reisnudeln</t>
@@ -222,10 +219,10 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.14"/>
   </cols>
@@ -272,7 +269,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -323,7 +320,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -340,7 +337,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -357,7 +354,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -374,7 +371,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -394,7 +391,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>7</v>
@@ -405,7 +402,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>400</v>
@@ -414,7 +411,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -422,7 +419,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1</v>
@@ -431,7 +428,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,7 +436,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>200</v>
@@ -448,7 +445,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,16 +453,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,7 +470,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>1</v>
@@ -482,7 +479,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,7 +487,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>80</v>
@@ -499,7 +496,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>